<commit_message>
README voor youtube links + Beoordeling Bas & Mike
</commit_message>
<xml_diff>
--- a/Project5 Beoordeling (1).xlsx
+++ b/Project5 Beoordeling (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://summacollege-my.sharepoint.com/personal/ps217498_summacollege_nl/Documents/school/Project 5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\SDleerjaar2\Projecten\Project 5\project5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{CE559A80-4A97-4A44-9513-F4068C60CBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A051C32-140E-4B12-8366-4181980F57D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30DCDF-1774-4A91-B505-A7E1EA26E6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11484" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>Groep1</t>
   </si>
@@ -851,37 +851,37 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="3.5546875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="7" width="3.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -898,7 +898,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -915,65 +915,91 @@
         <v>O</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="43.2" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="E11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -981,7 +1007,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -998,7 +1024,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="14" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1008,14 +1034,14 @@
       </c>
       <c r="F14" s="1" t="str">
         <f>UPPER(F52)</f>
-        <v/>
+        <v>V</v>
       </c>
       <c r="G14" s="1" t="str">
         <f>UPPER(G52)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1025,14 +1051,14 @@
       </c>
       <c r="F15" s="1" t="str">
         <f>F26</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G15" s="1" t="str">
         <f>G26</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1042,14 +1068,14 @@
       </c>
       <c r="F16" s="1" t="str">
         <f>F43</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G16" s="1" t="str">
         <f>G43</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1066,7 +1092,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="18" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1076,14 +1102,14 @@
       </c>
       <c r="F18" s="1" t="str">
         <f>IF(AND(F56="v",F67="v"),"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G18" s="1" t="str">
         <f>IF(AND(G56="v",G67="v"),"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1093,14 +1119,14 @@
       </c>
       <c r="F19" s="1" t="str">
         <f>UPPER(F53)</f>
-        <v/>
+        <v>O</v>
       </c>
       <c r="G19" s="1" t="str">
         <f>UPPER(G53)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1143,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="21" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1127,36 +1153,36 @@
       </c>
       <c r="F21" s="1" t="str">
         <f>IF(AND(F92="v",F95="v"),"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G21" s="1" t="str">
         <f>IF(AND(G92="v",G95="v"),"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>IF(E41="s","V",UPPER(E41))</f>
-        <v>V</v>
+        <v>O</v>
       </c>
       <c r="F22" s="1" t="str">
         <f>IF(F41="s","V",UPPER(F41))</f>
-        <v/>
+        <v>O</v>
       </c>
       <c r="G22" s="1" t="str">
         <f>IF(G41="s","V",UPPER(G41))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1166,14 +1192,14 @@
       </c>
       <c r="F26" s="8" t="str">
         <f t="shared" ref="F26:G26" si="0">IF(COUNTIF(F28:F37,"v")+COUNTIF(F28:F37,"s")=10,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1183,114 +1209,154 @@
       </c>
       <c r="F27" s="1" t="str">
         <f>IF(COUNTIF(F28:F30,"v")+COUNTIF(F28:F30,"s")=3,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G27" s="1" t="str">
         <f>IF(COUNTIF(G28:G30,"v")+COUNTIF(G28:G30,"s")=3,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -1300,44 +1366,56 @@
       </c>
       <c r="F38" s="8" t="str">
         <f t="shared" ref="F38:G38" si="1">IF(COUNTIF(F39:F40,"v")+COUNTIF(F39:F40,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G38" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
@@ -1347,14 +1425,14 @@
       </c>
       <c r="F43" s="8" t="str">
         <f>IF(COUNTIF(F45:F48,"v")+COUNTIF(F45:F48,"s")=4,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G43" s="8" t="str">
         <f>IF(COUNTIF(G45:G48,"v")+COUNTIF(G45:G48,"s")=4,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
@@ -1364,59 +1442,75 @@
       </c>
       <c r="F44" s="1" t="str">
         <f>IF(COUNTIF(F45:F46,"v")+COUNTIF(F45:F46,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G44" s="1" t="str">
         <f>IF(COUNTIF(G45:G46,"v")+COUNTIF(G45:G46,"s")=2,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F45" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F46" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F47" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>44</v>
       </c>
@@ -1426,39 +1520,47 @@
       </c>
       <c r="F51" s="8" t="str">
         <f>IF(AND(F52="v",F53="v"),"G",IF(F52="v","V","O"))</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G51" s="8" t="str">
         <f>IF(AND(G52="v",G53="v"),"G",IF(G52="v","V","O"))</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F52" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F53" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -1468,99 +1570,127 @@
       </c>
       <c r="F56" s="8" t="str">
         <f>IF(COUNTIF(F57:F66,"v")+COUNTIF(F57:F66,"s")=7,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G56" s="8" t="str">
         <f>IF(COUNTIF(G57:G66,"v")+COUNTIF(G57:G66,"s")=7,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F57" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C60" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F60" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F61" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C62" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F64" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F66" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -1570,39 +1700,47 @@
       </c>
       <c r="F67" s="1" t="str">
         <f>IF(COUNTIF(F68:F70,"v")+COUNTIF(F68:F70,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G67" s="1" t="str">
         <f>IF(COUNTIF(G68:G70,"v")+COUNTIF(G68:G70,"s")=2,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F68" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F70" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>63</v>
       </c>
@@ -1619,67 +1757,91 @@
         <v>O</v>
       </c>
     </row>
-    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-    </row>
-    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F73" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F74" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-    </row>
-    <row r="76" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F75" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-    </row>
-    <row r="77" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F76" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-    </row>
-    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F77" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F78" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
@@ -1689,109 +1851,141 @@
       </c>
       <c r="F79" s="1" t="str">
         <f>IF(COUNTIF(F80:F90,"v")+COUNTIF(F80:F90,"s")=8,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G79" s="1" t="str">
         <f>IF(COUNTIF(G80:G90,"v")+COUNTIF(G80:G90,"s")=8,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-    </row>
-    <row r="81" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F80" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-    </row>
-    <row r="82" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F81" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C83" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-    </row>
-    <row r="84" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F83" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C84" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
-    </row>
-    <row r="85" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F84" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C85" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-    </row>
-    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F85" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C87" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-    </row>
-    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F87" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C89" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-    </row>
-    <row r="90" spans="1:7" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F89" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C90" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F90" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E91" s="1" t="s">
         <v>79</v>
       </c>
@@ -1802,7 +1996,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>80</v>
       </c>
@@ -1812,34 +2006,42 @@
       </c>
       <c r="F92" s="1" t="str">
         <f>IF(COUNTIF(F93:F94,"v")+COUNTIF(F93:F94,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G92" s="1" t="str">
         <f>IF(COUNTIF(G93:G94,"v")+COUNTIF(G93:G94,"s")=2,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-    </row>
-    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F93" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F94" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>83</v>
       </c>
@@ -1849,32 +2051,40 @@
       </c>
       <c r="F95" s="1" t="str">
         <f>IF(COUNTIF(F96:F97,"v")+COUNTIF(F96:F97,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G95" s="1" t="str">
         <f>IF(COUNTIF(G96:G97,"v")+COUNTIF(G96:G97,"s")=2,"V","O")</f>
-        <v>O</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-    </row>
-    <row r="97" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F96" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
+      <c r="F97" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
@@ -1952,14 +2162,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1967,7 +2177,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1975,7 +2185,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Promo video link erbij + excl sheet bij gewerkt
</commit_message>
<xml_diff>
--- a/Project5 Beoordeling (1).xlsx
+++ b/Project5 Beoordeling (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\SDleerjaar2\Projecten\Project 5\project5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basbo\Desktop\project 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30DCDF-1774-4A91-B505-A7E1EA26E6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722A016D-9FB7-4D6F-A890-D1D9DF02372F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="92">
   <si>
     <t>Groep1</t>
   </si>
@@ -887,11 +887,11 @@
       </c>
       <c r="E4" s="6" t="str">
         <f>E17</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="F4" s="6" t="str">
         <f>F17</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G4" s="6" t="str">
         <f>G17</f>
@@ -904,11 +904,11 @@
       </c>
       <c r="E5" s="8" t="str">
         <f>IF(COUNTIF(E6:E12,"v")=7,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="F5" s="8" t="str">
         <f>IF(COUNTIF(F6:F12,"v")=7,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G5" s="8" t="str">
         <f>IF(COUNTIF(G6:G12,"v")=7,"V","O")</f>
@@ -1003,8 +1003,12 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1013,11 +1017,11 @@
       </c>
       <c r="E13" s="8" t="str">
         <f>IF(AND(E5="v",COUNTIF(E14:E16,"v")+COUNTIF(E14:E16,"g")=3),"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="F13" s="8" t="str">
         <f>IF(AND(F5="v",COUNTIF(F14:F16,"v")+COUNTIF(F14:F16,"g")=3),"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G13" s="8" t="str">
         <f>IF(AND(G5="v",COUNTIF(G14:G16,"v")+COUNTIF(G14:G16,"g")=3),"V","O")</f>
@@ -1081,11 +1085,11 @@
       </c>
       <c r="E17" s="8" t="str">
         <f>IF(COUNTIF(E18:E22,"v")=5,IF(E13="v","G",""),E13)</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="F17" s="8" t="str">
         <f>IF(COUNTIF(F18:F22,"v")=5,IF(F13="v","G",""),F13)</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G17" s="8" t="str">
         <f>IF(COUNTIF(G18:G22,"v")=5,IF(G13="v","G",""),G13)</f>

</xml_diff>

<commit_message>
README en beoordeling geupdate
</commit_message>
<xml_diff>
--- a/Project5 Beoordeling (1).xlsx
+++ b/Project5 Beoordeling (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\school\niv 4 mbo\Leerjaar 2\project 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basbo\Desktop\project 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A61A18-7977-44B6-8687-CA2657B10C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC401C5A-A080-4356-AD1F-E28A43CB2FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="92">
   <si>
     <t>Groep1</t>
   </si>
@@ -851,7 +851,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
       </c>
       <c r="G4" s="6" t="str">
         <f>G17</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
       </c>
       <c r="G5" s="8" t="str">
         <f>IF(COUNTIF(G6:G12,"v")=7,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,9 @@
       <c r="F12" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1025,7 +1027,7 @@
       </c>
       <c r="G13" s="8" t="str">
         <f>IF(AND(G5="v",COUNTIF(G14:G16,"v")+COUNTIF(G14:G16,"g")=3),"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="14" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -1093,7 +1095,7 @@
       </c>
       <c r="G17" s="8" t="str">
         <f>IF(COUNTIF(G18:G22,"v")=5,IF(G13="v","G",""),G13)</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="18" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">

</xml_diff>